<commit_message>
feat: Ajout des préconistions d'heures dans l'import Excel
</commit_message>
<xml_diff>
--- a/public/documents_gt/modele-import-referentiel-formation.xlsx
+++ b/public/documents_gt/modele-import-referentiel-formation.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/htdocs/redigeTonBut/public/documents_gt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A6817C-6FBA-F745-9AE9-45E79376D72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C7B2FF-9E19-3A4C-B074-2DB6C6C35F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{32BA1B02-F755-B948-B499-B8E429CA0EEC}"/>
+    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{32BA1B02-F755-B948-B499-B8E429CA0EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="1" r:id="rId1"/>
     <sheet name="SAE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Semestre</t>
   </si>
@@ -150,6 +149,15 @@
   </si>
   <si>
     <t>Test 2 d'une ressource</t>
+  </si>
+  <si>
+    <t>preco CM</t>
+  </si>
+  <si>
+    <t>Preco TD</t>
+  </si>
+  <si>
+    <t>Préco TP</t>
   </si>
 </sst>
 </file>
@@ -203,10 +211,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DFB4D0-669A-744B-99AD-CECD798C7791}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,7 +530,7 @@
     <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -581,8 +585,17 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -623,7 +636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -674,7 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A1FAB4-DEF9-174B-ACE7-7241C82BBE1B}">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>